<commit_message>
incorporate date of release into synapse_version
because NSCLC 2.0 came after NSCLC 2.1 release, sorting by version name to get the most recent version doesn't work. Had to add release date in order to consistently be able to get the most recent version of the data, regardless of the actual AACR naming convention
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laveryj\Desktop\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C105EF8F-60ED-4D32-92A5-4E23C4CC27BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7C4972-07B2-48E3-B580-A5AF062A06BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20745" yWindow="4965" windowWidth="21600" windowHeight="11385" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="98">
   <si>
     <t>cohort</t>
   </si>
@@ -307,6 +307,24 @@
   </si>
   <si>
     <t>syn24994179</t>
+  </si>
+  <si>
+    <t>release_date</t>
+  </si>
+  <si>
+    <t>2021-08</t>
+  </si>
+  <si>
+    <t>2022-05</t>
+  </si>
+  <si>
+    <t>2021-02</t>
+  </si>
+  <si>
+    <t>2021-10</t>
+  </si>
+  <si>
+    <t>2020-10</t>
   </si>
 </sst>
 </file>
@@ -667,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +699,7 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,8 +712,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -708,8 +729,11 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -722,8 +746,11 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -736,8 +763,11 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -750,8 +780,11 @@
       <c r="D5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -764,8 +797,11 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -778,8 +814,11 @@
       <c r="D7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -792,8 +831,11 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -806,8 +848,11 @@
       <c r="D9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -820,8 +865,11 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -834,8 +882,11 @@
       <c r="D11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -848,8 +899,11 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -862,8 +916,11 @@
       <c r="D13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -876,8 +933,11 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -890,8 +950,11 @@
       <c r="D15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -904,8 +967,11 @@
       <c r="D16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -918,8 +984,11 @@
       <c r="D17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -932,8 +1001,11 @@
       <c r="D18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -946,8 +1018,11 @@
       <c r="D19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -960,8 +1035,11 @@
       <c r="D20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -974,8 +1052,11 @@
       <c r="D21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -988,8 +1069,11 @@
       <c r="D22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1002,8 +1086,11 @@
       <c r="D23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1016,8 +1103,11 @@
       <c r="D24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1030,8 +1120,11 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1044,8 +1137,11 @@
       <c r="D26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1058,8 +1154,11 @@
       <c r="D27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1072,8 +1171,11 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1086,8 +1188,11 @@
       <c r="D29" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1100,8 +1205,11 @@
       <c r="D30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1114,8 +1222,11 @@
       <c r="D31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1128,8 +1239,11 @@
       <c r="D32" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1142,8 +1256,11 @@
       <c r="D33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1156,8 +1273,11 @@
       <c r="D34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1170,8 +1290,11 @@
       <c r="D35" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1184,8 +1307,11 @@
       <c r="D36" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1198,8 +1324,11 @@
       <c r="D37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1212,8 +1341,11 @@
       <c r="D38" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1226,8 +1358,11 @@
       <c r="D39" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1240,8 +1375,11 @@
       <c r="D40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1254,8 +1392,11 @@
       <c r="D41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1268,8 +1409,11 @@
       <c r="D42" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1282,8 +1426,11 @@
       <c r="D43" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1296,8 +1443,11 @@
       <c r="D44" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1310,8 +1460,11 @@
       <c r="D45" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1324,8 +1477,11 @@
       <c r="D46" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1338,8 +1494,11 @@
       <c r="D47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1352,8 +1511,11 @@
       <c r="D48" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1366,8 +1528,11 @@
       <c r="D49" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1380,8 +1545,11 @@
       <c r="D50" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1394,8 +1562,11 @@
       <c r="D51" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1408,8 +1579,11 @@
       <c r="D52" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1422,8 +1596,11 @@
       <c r="D53" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1436,8 +1613,11 @@
       <c r="D54" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1450,8 +1630,11 @@
       <c r="D55" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1464,8 +1647,11 @@
       <c r="D56" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1478,8 +1664,11 @@
       <c r="D57" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1492,8 +1681,11 @@
       <c r="D58" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -1506,8 +1698,11 @@
       <c r="D59" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -1520,8 +1715,11 @@
       <c r="D60" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -1534,8 +1732,11 @@
       <c r="D61" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1548,8 +1749,11 @@
       <c r="D62" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -1562,8 +1766,11 @@
       <c r="D63" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -1576,8 +1783,11 @@
       <c r="D64" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -1590,8 +1800,11 @@
       <c r="D65" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1604,8 +1817,11 @@
       <c r="D66" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1618,8 +1834,11 @@
       <c r="D67" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -1632,8 +1851,11 @@
       <c r="D68" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1646,8 +1868,11 @@
       <c r="D69" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -1659,6 +1884,9 @@
       </c>
       <c r="D70" t="s">
         <v>91</v>
+      </c>
+      <c r="E70" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CRC public v2 to list
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laveryj\Desktop\genieBPC\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7C4972-07B2-48E3-B580-A5AF062A06BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87AAC9A-A25A-43D8-96EA-F2D72E756E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="28680" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="116">
   <si>
     <t>cohort</t>
   </si>
@@ -325,13 +325,67 @@
   </si>
   <si>
     <t>2020-10</t>
+  </si>
+  <si>
+    <t>syn39802294</t>
+  </si>
+  <si>
+    <t>2022-10</t>
+  </si>
+  <si>
+    <t>syn39802300</t>
+  </si>
+  <si>
+    <t>syn39802305</t>
+  </si>
+  <si>
+    <t>syn39802310</t>
+  </si>
+  <si>
+    <t>syn39802316</t>
+  </si>
+  <si>
+    <t>syn39802321</t>
+  </si>
+  <si>
+    <t>syn39802324</t>
+  </si>
+  <si>
+    <t>syn39802332</t>
+  </si>
+  <si>
+    <t>syn39802339</t>
+  </si>
+  <si>
+    <t>2022-11</t>
+  </si>
+  <si>
+    <t>2022-12</t>
+  </si>
+  <si>
+    <t>2022-13</t>
+  </si>
+  <si>
+    <t>2022-14</t>
+  </si>
+  <si>
+    <t>2022-15</t>
+  </si>
+  <si>
+    <t>2022-16</t>
+  </si>
+  <si>
+    <t>2022-17</t>
+  </si>
+  <si>
+    <t>2022-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +397,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -685,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,7 +1949,161 @@
         <v>96</v>
       </c>
     </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>52</v>
+      </c>
+      <c r="B71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C78" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>106</v>
+      </c>
+      <c r="E78" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+      <c r="C79" t="s">
+        <v>53</v>
+      </c>
+      <c r="D79" t="s">
+        <v>107</v>
+      </c>
+      <c r="E79" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update synapse table all except Prostate
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87AAC9A-A25A-43D8-96EA-F2D72E756E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A366C312-9042-4674-9D50-7FE5563D5944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9024" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="140">
   <si>
     <t>cohort</t>
   </si>
@@ -360,25 +360,97 @@
     <t>2022-11</t>
   </si>
   <si>
-    <t>2022-12</t>
-  </si>
-  <si>
-    <t>2022-13</t>
-  </si>
-  <si>
-    <t>2022-14</t>
-  </si>
-  <si>
-    <t>2022-15</t>
-  </si>
-  <si>
-    <t>2022-16</t>
-  </si>
-  <si>
-    <t>2022-17</t>
-  </si>
-  <si>
-    <t>2022-18</t>
+    <t>PANC</t>
+  </si>
+  <si>
+    <t>syn47283351</t>
+  </si>
+  <si>
+    <t>syn47283323</t>
+  </si>
+  <si>
+    <t>syn47283590</t>
+  </si>
+  <si>
+    <t>syn47283470</t>
+  </si>
+  <si>
+    <t>syn47283544</t>
+  </si>
+  <si>
+    <t>syn47283508</t>
+  </si>
+  <si>
+    <t>syn47283390</t>
+  </si>
+  <si>
+    <t>syn47283430</t>
+  </si>
+  <si>
+    <t>syn47283628</t>
+  </si>
+  <si>
+    <t>Prostate</t>
+  </si>
+  <si>
+    <t>BLADDER</t>
+  </si>
+  <si>
+    <t>syn43172806</t>
+  </si>
+  <si>
+    <t>syn43172815</t>
+  </si>
+  <si>
+    <t>syn43172901</t>
+  </si>
+  <si>
+    <t>syn43172865</t>
+  </si>
+  <si>
+    <t>syn43172895</t>
+  </si>
+  <si>
+    <t>syn43172879</t>
+  </si>
+  <si>
+    <t>syn43172821</t>
+  </si>
+  <si>
+    <t>syn43172910</t>
+  </si>
+  <si>
+    <t>ca_radtx_dataset</t>
+  </si>
+  <si>
+    <t>syn44420748</t>
+  </si>
+  <si>
+    <t>syn44420702</t>
+  </si>
+  <si>
+    <t>syn44420708</t>
+  </si>
+  <si>
+    <t>syn44420744</t>
+  </si>
+  <si>
+    <t>syn44420731</t>
+  </si>
+  <si>
+    <t>syn44420739</t>
+  </si>
+  <si>
+    <t>syn44420737</t>
+  </si>
+  <si>
+    <t>syn44420719</t>
+  </si>
+  <si>
+    <t>syn44420726</t>
+  </si>
+  <si>
+    <t>2022-02</t>
   </si>
 </sst>
 </file>
@@ -745,21 +817,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89:E97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +848,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -793,7 +865,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -810,7 +882,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -827,7 +899,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -844,7 +916,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -861,7 +933,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -878,7 +950,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -895,7 +967,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -912,7 +984,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -929,7 +1001,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -946,7 +1018,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -963,7 +1035,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -980,7 +1052,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1069,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1014,7 +1086,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1031,7 +1103,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1048,7 +1120,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1137,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1082,7 +1154,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1099,7 +1171,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1116,7 +1188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1205,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1150,7 +1222,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1167,7 +1239,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1256,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1273,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1218,7 +1290,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1307,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1252,7 +1324,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1269,7 +1341,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1358,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1303,7 +1375,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1320,7 +1392,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1409,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1354,7 +1426,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1371,7 +1443,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1388,7 +1460,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1405,7 +1477,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1422,7 +1494,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1439,7 +1511,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1456,7 +1528,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1473,7 +1545,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1490,7 +1562,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1507,7 +1579,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1524,7 +1596,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1541,7 +1613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1558,7 +1630,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1575,7 +1647,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1592,7 +1664,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1609,7 +1681,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1626,7 +1698,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1643,7 +1715,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1660,7 +1732,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1677,7 +1749,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1694,7 +1766,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1711,7 +1783,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1728,7 +1800,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1745,7 +1817,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -1762,7 +1834,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -1779,7 +1851,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -1796,7 +1868,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1813,7 +1885,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -1830,7 +1902,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -1847,7 +1919,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -1864,7 +1936,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1881,7 +1953,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1898,7 +1970,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -1915,7 +1987,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -1932,7 +2004,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -1949,7 +2021,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -1966,7 +2038,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -1980,10 +2052,10 @@
         <v>100</v>
       </c>
       <c r="E72" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -1997,10 +2069,10 @@
         <v>101</v>
       </c>
       <c r="E73" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -2014,10 +2086,10 @@
         <v>102</v>
       </c>
       <c r="E74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2031,10 +2103,10 @@
         <v>103</v>
       </c>
       <c r="E75" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2048,10 +2120,10 @@
         <v>104</v>
       </c>
       <c r="E76" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2065,10 +2137,10 @@
         <v>105</v>
       </c>
       <c r="E77" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -2082,10 +2154,10 @@
         <v>106</v>
       </c>
       <c r="E78" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2099,7 +2171,565 @@
         <v>107</v>
       </c>
       <c r="E79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>111</v>
+      </c>
+      <c r="E80" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>110</v>
+      </c>
+      <c r="E81" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" t="s">
+        <v>12</v>
+      </c>
+      <c r="D82" t="s">
+        <v>112</v>
+      </c>
+      <c r="E82" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
         <v>115</v>
+      </c>
+      <c r="E85" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>109</v>
+      </c>
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>109</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" t="s">
+        <v>118</v>
+      </c>
+      <c r="E88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>119</v>
+      </c>
+      <c r="B90" t="s">
+        <v>22</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>119</v>
+      </c>
+      <c r="B93" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" t="s">
+        <v>129</v>
+      </c>
+      <c r="D98" t="s">
+        <v>130</v>
+      </c>
+      <c r="E98" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
+        <v>131</v>
+      </c>
+      <c r="E99" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>132</v>
+      </c>
+      <c r="E100" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>133</v>
+      </c>
+      <c r="E101" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" t="s">
+        <v>134</v>
+      </c>
+      <c r="E102" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>120</v>
+      </c>
+      <c r="B103" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>135</v>
+      </c>
+      <c r="E103" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>137</v>
+      </c>
+      <c r="E105" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>120</v>
+      </c>
+      <c r="B106" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" t="s">
+        <v>138</v>
+      </c>
+      <c r="E106" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" t="s">
+        <v>66</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
+        <v>121</v>
+      </c>
+      <c r="E107" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" t="s">
+        <v>66</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>122</v>
+      </c>
+      <c r="E108" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" t="s">
+        <v>66</v>
+      </c>
+      <c r="C109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" t="s">
+        <v>123</v>
+      </c>
+      <c r="E109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" t="s">
+        <v>66</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" t="s">
+        <v>124</v>
+      </c>
+      <c r="E110" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" t="s">
+        <v>66</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D111" t="s">
+        <v>125</v>
+      </c>
+      <c r="E111" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" t="s">
+        <v>66</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>126</v>
+      </c>
+      <c r="E112" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" t="s">
+        <v>66</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>127</v>
+      </c>
+      <c r="E113" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" t="s">
+        <v>66</v>
+      </c>
+      <c r="C114" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" t="s">
+        <v>127</v>
+      </c>
+      <c r="E114" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" t="s">
+        <v>66</v>
+      </c>
+      <c r="C115" t="s">
+        <v>53</v>
+      </c>
+      <c r="D115" t="s">
+        <v>128</v>
+      </c>
+      <c r="E115" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all except prostate
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A366C312-9042-4674-9D50-7FE5563D5944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A458E1-2A1C-4EDF-9C63-00862541D51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9024" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="29970" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="139">
   <si>
     <t>cohort</t>
   </si>
@@ -388,9 +388,6 @@
   </si>
   <si>
     <t>syn47283628</t>
-  </si>
-  <si>
-    <t>Prostate</t>
   </si>
   <si>
     <t>BLADDER</t>
@@ -817,21 +814,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89:E97"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +845,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -865,7 +862,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -882,7 +879,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -899,7 +896,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -916,7 +913,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -933,7 +930,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -950,7 +947,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -967,7 +964,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -984,7 +981,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1069,7 +1066,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1086,7 +1083,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1117,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +1134,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1154,7 +1151,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1171,7 +1168,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1188,7 +1185,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1202,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1219,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1236,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1273,7 +1270,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1287,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1307,7 +1304,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1324,7 +1321,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1355,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1375,7 +1372,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1409,7 +1406,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1426,7 +1423,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1477,7 +1474,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1494,7 +1491,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1511,7 +1508,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1528,7 +1525,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1545,7 +1542,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1562,7 +1559,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1579,7 +1576,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1596,7 +1593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1613,7 +1610,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1647,7 +1644,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1698,7 +1695,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1715,7 +1712,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1732,7 +1729,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1749,7 +1746,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1783,7 +1780,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1800,7 +1797,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1817,7 +1814,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -1834,7 +1831,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -1851,7 +1848,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -1868,7 +1865,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1885,7 +1882,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -1902,7 +1899,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -1919,7 +1916,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -1936,7 +1933,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -1953,7 +1950,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -1987,7 +1984,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2004,7 +2001,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2021,7 +2018,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -2038,7 +2035,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -2055,7 +2052,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -2072,7 +2069,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -2089,7 +2086,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2106,7 +2103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2123,7 +2120,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2140,7 +2137,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -2157,7 +2154,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2174,7 +2171,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>109</v>
       </c>
@@ -2188,10 +2185,10 @@
         <v>111</v>
       </c>
       <c r="E80" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>109</v>
       </c>
@@ -2205,10 +2202,10 @@
         <v>110</v>
       </c>
       <c r="E81" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>109</v>
       </c>
@@ -2222,10 +2219,10 @@
         <v>112</v>
       </c>
       <c r="E82" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>109</v>
       </c>
@@ -2239,10 +2236,10 @@
         <v>113</v>
       </c>
       <c r="E83" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>109</v>
       </c>
@@ -2256,10 +2253,10 @@
         <v>114</v>
       </c>
       <c r="E84" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -2273,10 +2270,10 @@
         <v>115</v>
       </c>
       <c r="E85" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>109</v>
       </c>
@@ -2290,10 +2287,10 @@
         <v>116</v>
       </c>
       <c r="E86" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>109</v>
       </c>
@@ -2307,10 +2304,10 @@
         <v>117</v>
       </c>
       <c r="E87" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>109</v>
       </c>
@@ -2324,10 +2321,10 @@
         <v>118</v>
       </c>
       <c r="E88" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>119</v>
       </c>
@@ -2335,10 +2332,16 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="D89" t="s">
+        <v>129</v>
+      </c>
+      <c r="E89" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -2346,10 +2349,16 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>119</v>
       </c>
@@ -2357,10 +2366,16 @@
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>131</v>
+      </c>
+      <c r="E91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>119</v>
       </c>
@@ -2368,10 +2383,16 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="D92" t="s">
+        <v>132</v>
+      </c>
+      <c r="E92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>119</v>
       </c>
@@ -2379,10 +2400,16 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>133</v>
+      </c>
+      <c r="E93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>119</v>
       </c>
@@ -2390,10 +2417,16 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D94" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>119</v>
       </c>
@@ -2401,10 +2434,16 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>135</v>
+      </c>
+      <c r="E95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>119</v>
       </c>
@@ -2412,10 +2451,16 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>136</v>
+      </c>
+      <c r="E96" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>119</v>
       </c>
@@ -2423,312 +2468,165 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" t="s">
+        <v>137</v>
+      </c>
+      <c r="E97" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>120</v>
+      </c>
+      <c r="E98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>121</v>
+      </c>
+      <c r="E99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>122</v>
+      </c>
+      <c r="E100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" t="s">
+        <v>66</v>
+      </c>
+      <c r="C101" t="s">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>123</v>
+      </c>
+      <c r="E101" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" t="s">
+        <v>66</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>124</v>
+      </c>
+      <c r="E102" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" t="s">
+        <v>66</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="s">
+        <v>126</v>
+      </c>
+      <c r="E104" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" t="s">
+        <v>126</v>
+      </c>
+      <c r="E105" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" t="s">
+        <v>66</v>
+      </c>
+      <c r="C106" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>120</v>
-      </c>
-      <c r="B98" t="s">
-        <v>22</v>
-      </c>
-      <c r="C98" t="s">
-        <v>129</v>
-      </c>
-      <c r="D98" t="s">
-        <v>130</v>
-      </c>
-      <c r="E98" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>120</v>
-      </c>
-      <c r="B99" t="s">
-        <v>22</v>
-      </c>
-      <c r="C99" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" t="s">
-        <v>131</v>
-      </c>
-      <c r="E99" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>120</v>
-      </c>
-      <c r="B100" t="s">
-        <v>22</v>
-      </c>
-      <c r="C100" t="s">
-        <v>7</v>
-      </c>
-      <c r="D100" t="s">
-        <v>132</v>
-      </c>
-      <c r="E100" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" t="s">
-        <v>22</v>
-      </c>
-      <c r="C101" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" t="s">
-        <v>133</v>
-      </c>
-      <c r="E101" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>120</v>
-      </c>
-      <c r="B102" t="s">
-        <v>22</v>
-      </c>
-      <c r="C102" t="s">
-        <v>8</v>
-      </c>
-      <c r="D102" t="s">
-        <v>134</v>
-      </c>
-      <c r="E102" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>120</v>
-      </c>
-      <c r="B103" t="s">
-        <v>22</v>
-      </c>
-      <c r="C103" t="s">
-        <v>10</v>
-      </c>
-      <c r="D103" t="s">
-        <v>135</v>
-      </c>
-      <c r="E103" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>120</v>
-      </c>
-      <c r="B104" t="s">
-        <v>22</v>
-      </c>
-      <c r="C104" t="s">
-        <v>9</v>
-      </c>
-      <c r="D104" t="s">
-        <v>136</v>
-      </c>
-      <c r="E104" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>120</v>
-      </c>
-      <c r="B105" t="s">
-        <v>22</v>
-      </c>
-      <c r="C105" t="s">
-        <v>5</v>
-      </c>
-      <c r="D105" t="s">
-        <v>137</v>
-      </c>
-      <c r="E105" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" t="s">
-        <v>22</v>
-      </c>
-      <c r="C106" t="s">
-        <v>11</v>
-      </c>
       <c r="D106" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E106" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>79</v>
-      </c>
-      <c r="B107" t="s">
-        <v>66</v>
-      </c>
-      <c r="C107" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" t="s">
-        <v>121</v>
-      </c>
-      <c r="E107" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>79</v>
-      </c>
-      <c r="B108" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" t="s">
-        <v>7</v>
-      </c>
-      <c r="D108" t="s">
-        <v>122</v>
-      </c>
-      <c r="E108" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>79</v>
-      </c>
-      <c r="B109" t="s">
-        <v>66</v>
-      </c>
-      <c r="C109" t="s">
-        <v>12</v>
-      </c>
-      <c r="D109" t="s">
-        <v>123</v>
-      </c>
-      <c r="E109" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>79</v>
-      </c>
-      <c r="B110" t="s">
-        <v>66</v>
-      </c>
-      <c r="C110" t="s">
-        <v>8</v>
-      </c>
-      <c r="D110" t="s">
-        <v>124</v>
-      </c>
-      <c r="E110" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>79</v>
-      </c>
-      <c r="B111" t="s">
-        <v>66</v>
-      </c>
-      <c r="C111" t="s">
-        <v>10</v>
-      </c>
-      <c r="D111" t="s">
-        <v>125</v>
-      </c>
-      <c r="E111" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>79</v>
-      </c>
-      <c r="B112" t="s">
-        <v>66</v>
-      </c>
-      <c r="C112" t="s">
-        <v>9</v>
-      </c>
-      <c r="D112" t="s">
-        <v>126</v>
-      </c>
-      <c r="E112" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>79</v>
-      </c>
-      <c r="B113" t="s">
-        <v>66</v>
-      </c>
-      <c r="C113" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" t="s">
-        <v>127</v>
-      </c>
-      <c r="E113" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>79</v>
-      </c>
-      <c r="B114" t="s">
-        <v>66</v>
-      </c>
-      <c r="C114" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114" t="s">
-        <v>127</v>
-      </c>
-      <c r="E114" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>79</v>
-      </c>
-      <c r="B115" t="s">
-        <v>66</v>
-      </c>
-      <c r="C115" t="s">
-        <v>53</v>
-      </c>
-      <c r="D115" t="s">
-        <v>128</v>
-      </c>
-      <c r="E115" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PANC and prostate v1.2 consortium
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFC4C3F-8C25-4FF7-ACD0-D38FCCF10536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E0748B-5E1E-4879-97F1-67A7788D4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="173">
   <si>
     <t>cohort</t>
   </si>
@@ -484,6 +484,72 @@
   </si>
   <si>
     <t>syn50895319</t>
+  </si>
+  <si>
+    <t>2023-01</t>
+  </si>
+  <si>
+    <t>syn50908650</t>
+  </si>
+  <si>
+    <t>syn50908651</t>
+  </si>
+  <si>
+    <t>syn50908652</t>
+  </si>
+  <si>
+    <t>syn50908653</t>
+  </si>
+  <si>
+    <t>syn50908654</t>
+  </si>
+  <si>
+    <t>syn50908655</t>
+  </si>
+  <si>
+    <t>syn50908656</t>
+  </si>
+  <si>
+    <t>syn50908657</t>
+  </si>
+  <si>
+    <t>syn50908658</t>
+  </si>
+  <si>
+    <t>syn50908659</t>
+  </si>
+  <si>
+    <t>syn50908660</t>
+  </si>
+  <si>
+    <t>syn50908661</t>
+  </si>
+  <si>
+    <t>syn50908662</t>
+  </si>
+  <si>
+    <t>syn50908663</t>
+  </si>
+  <si>
+    <t>syn50908664</t>
+  </si>
+  <si>
+    <t>syn50908665</t>
+  </si>
+  <si>
+    <t>syn50908666</t>
+  </si>
+  <si>
+    <t>syn50908667</t>
+  </si>
+  <si>
+    <t>syn50908668</t>
+  </si>
+  <si>
+    <t>syn50908669</t>
+  </si>
+  <si>
+    <t>syn43172837</t>
   </si>
 </sst>
 </file>
@@ -533,9 +599,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G111" sqref="G111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,7 +2710,7 @@
         <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="E105" t="s">
         <v>99</v>
@@ -2834,6 +2901,346 @@
       </c>
       <c r="E116" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>109</v>
+      </c>
+      <c r="B117" t="s">
+        <v>66</v>
+      </c>
+      <c r="C117" t="s">
+        <v>128</v>
+      </c>
+      <c r="D117" t="s">
+        <v>152</v>
+      </c>
+      <c r="E117" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>109</v>
+      </c>
+      <c r="B118" t="s">
+        <v>66</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E118" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>109</v>
+      </c>
+      <c r="B119" t="s">
+        <v>66</v>
+      </c>
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" t="s">
+        <v>154</v>
+      </c>
+      <c r="E119" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>109</v>
+      </c>
+      <c r="B120" t="s">
+        <v>66</v>
+      </c>
+      <c r="C120" t="s">
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>155</v>
+      </c>
+      <c r="E120" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>109</v>
+      </c>
+      <c r="B121" t="s">
+        <v>66</v>
+      </c>
+      <c r="C121" t="s">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>156</v>
+      </c>
+      <c r="E121" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>109</v>
+      </c>
+      <c r="B122" t="s">
+        <v>66</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122" t="s">
+        <v>157</v>
+      </c>
+      <c r="E122" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>109</v>
+      </c>
+      <c r="B123" t="s">
+        <v>66</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>158</v>
+      </c>
+      <c r="E123" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>109</v>
+      </c>
+      <c r="B124" t="s">
+        <v>66</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" t="s">
+        <v>159</v>
+      </c>
+      <c r="E124" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" t="s">
+        <v>66</v>
+      </c>
+      <c r="C125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>160</v>
+      </c>
+      <c r="E125" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>109</v>
+      </c>
+      <c r="B126" t="s">
+        <v>66</v>
+      </c>
+      <c r="C126" t="s">
+        <v>53</v>
+      </c>
+      <c r="D126" t="s">
+        <v>161</v>
+      </c>
+      <c r="E126" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>139</v>
+      </c>
+      <c r="B127" t="s">
+        <v>66</v>
+      </c>
+      <c r="C127" t="s">
+        <v>128</v>
+      </c>
+      <c r="D127" t="s">
+        <v>162</v>
+      </c>
+      <c r="E127" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>139</v>
+      </c>
+      <c r="B128" t="s">
+        <v>66</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
+        <v>163</v>
+      </c>
+      <c r="E128" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>139</v>
+      </c>
+      <c r="B129" t="s">
+        <v>66</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" t="s">
+        <v>164</v>
+      </c>
+      <c r="E129" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>139</v>
+      </c>
+      <c r="B130" t="s">
+        <v>66</v>
+      </c>
+      <c r="C130" t="s">
+        <v>12</v>
+      </c>
+      <c r="D130" t="s">
+        <v>165</v>
+      </c>
+      <c r="E130" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>139</v>
+      </c>
+      <c r="B131" t="s">
+        <v>66</v>
+      </c>
+      <c r="C131" t="s">
+        <v>8</v>
+      </c>
+      <c r="D131" t="s">
+        <v>166</v>
+      </c>
+      <c r="E131" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>139</v>
+      </c>
+      <c r="B132" t="s">
+        <v>66</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" t="s">
+        <v>167</v>
+      </c>
+      <c r="E132" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>139</v>
+      </c>
+      <c r="B133" t="s">
+        <v>66</v>
+      </c>
+      <c r="C133" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" t="s">
+        <v>168</v>
+      </c>
+      <c r="E133" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>139</v>
+      </c>
+      <c r="B134" t="s">
+        <v>66</v>
+      </c>
+      <c r="C134" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="s">
+        <v>169</v>
+      </c>
+      <c r="E134" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>139</v>
+      </c>
+      <c r="B135" t="s">
+        <v>66</v>
+      </c>
+      <c r="C135" t="s">
+        <v>11</v>
+      </c>
+      <c r="D135" t="s">
+        <v>170</v>
+      </c>
+      <c r="E135" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>139</v>
+      </c>
+      <c r="B136" t="s">
+        <v>66</v>
+      </c>
+      <c r="C136" t="s">
+        <v>53</v>
+      </c>
+      <c r="D136" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cbioportal files for CRC
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E0748B-5E1E-4879-97F1-67A7788D4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56131950-F8B5-400D-BFDD-5BEA15E72D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="28680" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="176">
   <si>
     <t>cohort</t>
   </si>
@@ -550,6 +550,15 @@
   </si>
   <si>
     <t>syn43172837</t>
+  </si>
+  <si>
+    <t>syn30381335</t>
+  </si>
+  <si>
+    <t>syn30381332</t>
+  </si>
+  <si>
+    <t>syn30381327</t>
   </si>
 </sst>
 </file>
@@ -917,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E136"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,16 +2268,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="E79" t="s">
         <v>99</v>
@@ -2276,53 +2285,53 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="E80" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D81" t="s">
-        <v>110</v>
+        <v>175</v>
       </c>
       <c r="E81" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D82" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E82" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2333,10 +2342,10 @@
         <v>22</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E83" t="s">
         <v>138</v>
@@ -2350,10 +2359,10 @@
         <v>22</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E84" t="s">
         <v>138</v>
@@ -2367,10 +2376,10 @@
         <v>22</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D85" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E85" t="s">
         <v>138</v>
@@ -2384,10 +2393,10 @@
         <v>22</v>
       </c>
       <c r="C86" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E86" t="s">
         <v>138</v>
@@ -2401,10 +2410,10 @@
         <v>22</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E87" t="s">
         <v>138</v>
@@ -2418,10 +2427,10 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E88" t="s">
         <v>138</v>
@@ -2429,53 +2438,53 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s">
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E89" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B90" t="s">
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E90" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D91" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E91" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,10 +2495,10 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D92" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E92" t="s">
         <v>108</v>
@@ -2503,10 +2512,10 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E93" t="s">
         <v>108</v>
@@ -2520,10 +2529,10 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D94" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E94" t="s">
         <v>108</v>
@@ -2537,10 +2546,10 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E95" t="s">
         <v>108</v>
@@ -2554,10 +2563,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D96" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E96" t="s">
         <v>108</v>
@@ -2571,10 +2580,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -2582,53 +2591,53 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D98" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E98" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E99" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E100" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2639,10 +2648,10 @@
         <v>66</v>
       </c>
       <c r="C101" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D101" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E101" t="s">
         <v>99</v>
@@ -2656,10 +2665,10 @@
         <v>66</v>
       </c>
       <c r="C102" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D102" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E102" t="s">
         <v>99</v>
@@ -2673,10 +2682,10 @@
         <v>66</v>
       </c>
       <c r="C103" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D103" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E103" t="s">
         <v>99</v>
@@ -2690,10 +2699,10 @@
         <v>66</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D104" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E104" t="s">
         <v>99</v>
@@ -2707,10 +2716,10 @@
         <v>66</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D105" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="E105" t="s">
         <v>99</v>
@@ -2724,10 +2733,10 @@
         <v>66</v>
       </c>
       <c r="C106" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E106" t="s">
         <v>99</v>
@@ -2735,53 +2744,53 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B107" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C107" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="D107" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E107" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B108" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C108" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="E108" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B109" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C109" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D109" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E109" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,10 +2801,10 @@
         <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D110" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E110" t="s">
         <v>140</v>
@@ -2809,10 +2818,10 @@
         <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D111" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E111" t="s">
         <v>140</v>
@@ -2826,10 +2835,10 @@
         <v>22</v>
       </c>
       <c r="C112" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D112" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E112" t="s">
         <v>140</v>
@@ -2843,10 +2852,10 @@
         <v>22</v>
       </c>
       <c r="C113" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D113" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E113" t="s">
         <v>140</v>
@@ -2860,10 +2869,10 @@
         <v>22</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E114" t="s">
         <v>140</v>
@@ -2877,10 +2886,10 @@
         <v>22</v>
       </c>
       <c r="C115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E115" t="s">
         <v>140</v>
@@ -2894,10 +2903,10 @@
         <v>22</v>
       </c>
       <c r="C116" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D116" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E116" t="s">
         <v>140</v>
@@ -2905,53 +2914,53 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C117" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E117" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B118" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C118" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>153</v>
+        <v>11</v>
+      </c>
+      <c r="D118" t="s">
+        <v>149</v>
       </c>
       <c r="E118" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C119" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D119" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E119" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2962,10 +2971,10 @@
         <v>66</v>
       </c>
       <c r="C120" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D120" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E120" t="s">
         <v>151</v>
@@ -2979,10 +2988,10 @@
         <v>66</v>
       </c>
       <c r="C121" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" t="s">
-        <v>156</v>
+        <v>6</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E121" t="s">
         <v>151</v>
@@ -2996,10 +3005,10 @@
         <v>66</v>
       </c>
       <c r="C122" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E122" t="s">
         <v>151</v>
@@ -3013,10 +3022,10 @@
         <v>66</v>
       </c>
       <c r="C123" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E123" t="s">
         <v>151</v>
@@ -3030,10 +3039,10 @@
         <v>66</v>
       </c>
       <c r="C124" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E124" t="s">
         <v>151</v>
@@ -3047,10 +3056,10 @@
         <v>66</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E125" t="s">
         <v>151</v>
@@ -3064,10 +3073,10 @@
         <v>66</v>
       </c>
       <c r="C126" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="D126" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E126" t="s">
         <v>151</v>
@@ -3075,16 +3084,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B127" t="s">
         <v>66</v>
       </c>
       <c r="C127" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E127" t="s">
         <v>151</v>
@@ -3092,16 +3101,16 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B128" t="s">
         <v>66</v>
       </c>
       <c r="C128" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D128" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E128" t="s">
         <v>151</v>
@@ -3109,16 +3118,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B129" t="s">
         <v>66</v>
       </c>
       <c r="C129" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D129" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E129" t="s">
         <v>151</v>
@@ -3132,10 +3141,10 @@
         <v>66</v>
       </c>
       <c r="C130" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D130" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E130" t="s">
         <v>151</v>
@@ -3149,10 +3158,10 @@
         <v>66</v>
       </c>
       <c r="C131" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E131" t="s">
         <v>151</v>
@@ -3166,10 +3175,10 @@
         <v>66</v>
       </c>
       <c r="C132" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D132" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E132" t="s">
         <v>151</v>
@@ -3183,10 +3192,10 @@
         <v>66</v>
       </c>
       <c r="C133" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D133" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E133" t="s">
         <v>151</v>
@@ -3200,10 +3209,10 @@
         <v>66</v>
       </c>
       <c r="C134" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D134" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E134" t="s">
         <v>151</v>
@@ -3217,10 +3226,10 @@
         <v>66</v>
       </c>
       <c r="C135" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D135" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E135" t="s">
         <v>151</v>
@@ -3234,12 +3243,63 @@
         <v>66</v>
       </c>
       <c r="C136" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" t="s">
+        <v>168</v>
+      </c>
+      <c r="E136" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>139</v>
+      </c>
+      <c r="B137" t="s">
+        <v>66</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137" t="s">
+        <v>169</v>
+      </c>
+      <c r="E137" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" t="s">
+        <v>66</v>
+      </c>
+      <c r="C138" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" t="s">
+        <v>170</v>
+      </c>
+      <c r="E138" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>66</v>
+      </c>
+      <c r="C139" t="s">
         <v>53</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D139" t="s">
         <v>171</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E139" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
error fix in xlsx file
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56131950-F8B5-400D-BFDD-5BEA15E72D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC89C04-EC55-408A-B1C4-31DD389B2E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
   <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B80" t="s">
         <v>21</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
genetic data from cbp
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\FuchsH\Projects\GENIEBPC\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC89C04-EC55-408A-B1C4-31DD389B2E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814369D9-99E8-4F68-916E-D7EF90356336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1515" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="194">
   <si>
     <t>cohort</t>
   </si>
@@ -559,6 +559,60 @@
   </si>
   <si>
     <t>syn30381327</t>
+  </si>
+  <si>
+    <t>syn26349094</t>
+  </si>
+  <si>
+    <t>syn26349091</t>
+  </si>
+  <si>
+    <t>syn26349092</t>
+  </si>
+  <si>
+    <t>syn50697875</t>
+  </si>
+  <si>
+    <t>syn50697871</t>
+  </si>
+  <si>
+    <t>syn50697855</t>
+  </si>
+  <si>
+    <t>syn26990191</t>
+  </si>
+  <si>
+    <t>syn26990193</t>
+  </si>
+  <si>
+    <t>syn26990176</t>
+  </si>
+  <si>
+    <t>syn32299096</t>
+  </si>
+  <si>
+    <t>syn32299105</t>
+  </si>
+  <si>
+    <t>syn32299128</t>
+  </si>
+  <si>
+    <t>syn26475434</t>
+  </si>
+  <si>
+    <t>syn26475436</t>
+  </si>
+  <si>
+    <t>syn26475433</t>
+  </si>
+  <si>
+    <t>syn50697700</t>
+  </si>
+  <si>
+    <t>syn50697696</t>
+  </si>
+  <si>
+    <t>syn50697680</t>
   </si>
 </sst>
 </file>
@@ -926,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79:A81"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,6 +992,8 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2274,10 +2330,10 @@
         <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="E79" t="s">
         <v>99</v>
@@ -2291,10 +2347,10 @@
         <v>21</v>
       </c>
       <c r="C80" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E80" t="s">
         <v>99</v>
@@ -2308,10 +2364,10 @@
         <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E81" t="s">
         <v>99</v>
@@ -2325,10 +2381,10 @@
         <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="E82" t="s">
         <v>99</v>
@@ -2489,53 +2545,53 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B92" t="s">
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="D92" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="E92" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D93" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="E93" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" t="s">
-        <v>131</v>
+        <v>36</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="E94" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,10 +2602,10 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D95" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E95" t="s">
         <v>108</v>
@@ -2563,10 +2619,10 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E96" t="s">
         <v>108</v>
@@ -2580,10 +2636,10 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E97" t="s">
         <v>108</v>
@@ -2597,10 +2653,10 @@
         <v>22</v>
       </c>
       <c r="C98" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D98" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E98" t="s">
         <v>108</v>
@@ -2614,10 +2670,10 @@
         <v>22</v>
       </c>
       <c r="C99" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D99" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E99" t="s">
         <v>108</v>
@@ -2631,10 +2687,10 @@
         <v>22</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D100" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E100" t="s">
         <v>108</v>
@@ -2642,104 +2698,104 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B101" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="E101" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B102" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D102" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="E102" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B103" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D103" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="E103" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C104" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D104" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="E104" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B105" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D105" t="s">
-        <v>124</v>
+        <v>182</v>
       </c>
       <c r="E105" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="E106" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,10 +2806,10 @@
         <v>66</v>
       </c>
       <c r="C107" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D107" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E107" t="s">
         <v>99</v>
@@ -2767,10 +2823,10 @@
         <v>66</v>
       </c>
       <c r="C108" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D108" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
       <c r="E108" t="s">
         <v>99</v>
@@ -2784,10 +2840,10 @@
         <v>66</v>
       </c>
       <c r="C109" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="D109" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E109" t="s">
         <v>99</v>
@@ -2795,155 +2851,155 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B110" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C110" t="s">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D110" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="E110" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B111" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C111" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D111" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="E111" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B112" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C112" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D112" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="E112" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B113" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C113" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="E113" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B114" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C114" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D114" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="E114" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B115" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C115" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D115" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="E115" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B116" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C116" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D116" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="E116" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B117" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C117" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D117" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="E117" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="B118" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C118" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D118" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="E118" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2954,10 +3010,10 @@
         <v>22</v>
       </c>
       <c r="C119" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D119" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E119" t="s">
         <v>140</v>
@@ -2965,172 +3021,172 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B120" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E120" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C121" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>153</v>
+        <v>7</v>
+      </c>
+      <c r="D121" t="s">
+        <v>143</v>
       </c>
       <c r="E121" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C122" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E122" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B123" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C123" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D123" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E123" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B124" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C124" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D124" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E124" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B125" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D125" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E125" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B126" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C126" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D126" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E126" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C127" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D127" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E127" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B128" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="D128" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E128" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B129" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C129" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D129" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="E129" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3138,16 +3194,16 @@
         <v>139</v>
       </c>
       <c r="B130" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C130" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="D130" t="s">
-        <v>162</v>
+        <v>188</v>
       </c>
       <c r="E130" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3155,30 +3211,30 @@
         <v>139</v>
       </c>
       <c r="B131" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="D131" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
       <c r="E131" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B132" t="s">
         <v>66</v>
       </c>
       <c r="C132" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="D132" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E132" t="s">
         <v>151</v>
@@ -3186,16 +3242,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B133" t="s">
         <v>66</v>
       </c>
       <c r="C133" t="s">
-        <v>12</v>
-      </c>
-      <c r="D133" t="s">
-        <v>165</v>
+        <v>6</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E133" t="s">
         <v>151</v>
@@ -3203,16 +3259,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B134" t="s">
         <v>66</v>
       </c>
       <c r="C134" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D134" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="E134" t="s">
         <v>151</v>
@@ -3220,16 +3276,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B135" t="s">
         <v>66</v>
       </c>
       <c r="C135" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E135" t="s">
         <v>151</v>
@@ -3237,16 +3293,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B136" t="s">
         <v>66</v>
       </c>
       <c r="C136" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D136" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E136" t="s">
         <v>151</v>
@@ -3254,16 +3310,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B137" t="s">
         <v>66</v>
       </c>
       <c r="C137" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D137" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E137" t="s">
         <v>151</v>
@@ -3271,16 +3327,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="B138" t="s">
         <v>66</v>
       </c>
       <c r="C138" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D138" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E138" t="s">
         <v>151</v>
@@ -3288,18 +3344,324 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>109</v>
+      </c>
+      <c r="B139" t="s">
+        <v>66</v>
+      </c>
+      <c r="C139" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" t="s">
+        <v>159</v>
+      </c>
+      <c r="E139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>109</v>
+      </c>
+      <c r="B140" t="s">
+        <v>66</v>
+      </c>
+      <c r="C140" t="s">
+        <v>11</v>
+      </c>
+      <c r="D140" t="s">
+        <v>160</v>
+      </c>
+      <c r="E140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>109</v>
+      </c>
+      <c r="B141" t="s">
+        <v>66</v>
+      </c>
+      <c r="C141" t="s">
+        <v>53</v>
+      </c>
+      <c r="D141" t="s">
+        <v>161</v>
+      </c>
+      <c r="E141" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>109</v>
+      </c>
+      <c r="B142" t="s">
+        <v>66</v>
+      </c>
+      <c r="C142" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142" t="s">
+        <v>180</v>
+      </c>
+      <c r="E142" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>109</v>
+      </c>
+      <c r="B143" t="s">
+        <v>66</v>
+      </c>
+      <c r="C143" t="s">
+        <v>34</v>
+      </c>
+      <c r="D143" t="s">
+        <v>179</v>
+      </c>
+      <c r="E143" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>109</v>
+      </c>
+      <c r="B144" t="s">
+        <v>66</v>
+      </c>
+      <c r="C144" t="s">
+        <v>36</v>
+      </c>
+      <c r="D144" t="s">
+        <v>181</v>
+      </c>
+      <c r="E144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>139</v>
       </c>
-      <c r="B139" t="s">
-        <v>66</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="B145" t="s">
+        <v>66</v>
+      </c>
+      <c r="C145" t="s">
+        <v>128</v>
+      </c>
+      <c r="D145" t="s">
+        <v>162</v>
+      </c>
+      <c r="E145" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>139</v>
+      </c>
+      <c r="B146" t="s">
+        <v>66</v>
+      </c>
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" t="s">
+        <v>163</v>
+      </c>
+      <c r="E146" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>139</v>
+      </c>
+      <c r="B147" t="s">
+        <v>66</v>
+      </c>
+      <c r="C147" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" t="s">
+        <v>164</v>
+      </c>
+      <c r="E147" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>139</v>
+      </c>
+      <c r="B148" t="s">
+        <v>66</v>
+      </c>
+      <c r="C148" t="s">
+        <v>12</v>
+      </c>
+      <c r="D148" t="s">
+        <v>165</v>
+      </c>
+      <c r="E148" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>139</v>
+      </c>
+      <c r="B149" t="s">
+        <v>66</v>
+      </c>
+      <c r="C149" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" t="s">
+        <v>166</v>
+      </c>
+      <c r="E149" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150" t="s">
+        <v>66</v>
+      </c>
+      <c r="C150" t="s">
+        <v>10</v>
+      </c>
+      <c r="D150" t="s">
+        <v>167</v>
+      </c>
+      <c r="E150" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>139</v>
+      </c>
+      <c r="B151" t="s">
+        <v>66</v>
+      </c>
+      <c r="C151" t="s">
+        <v>9</v>
+      </c>
+      <c r="D151" t="s">
+        <v>168</v>
+      </c>
+      <c r="E151" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>139</v>
+      </c>
+      <c r="B152" t="s">
+        <v>66</v>
+      </c>
+      <c r="C152" t="s">
+        <v>5</v>
+      </c>
+      <c r="D152" t="s">
+        <v>169</v>
+      </c>
+      <c r="E152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>139</v>
+      </c>
+      <c r="B153" t="s">
+        <v>66</v>
+      </c>
+      <c r="C153" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" t="s">
+        <v>170</v>
+      </c>
+      <c r="E153" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154" t="s">
+        <v>66</v>
+      </c>
+      <c r="C154" t="s">
         <v>53</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D154" t="s">
         <v>171</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E154" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>139</v>
+      </c>
+      <c r="B155" t="s">
+        <v>66</v>
+      </c>
+      <c r="C155" t="s">
+        <v>32</v>
+      </c>
+      <c r="D155" t="s">
+        <v>192</v>
+      </c>
+      <c r="E155" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>139</v>
+      </c>
+      <c r="B156" t="s">
+        <v>66</v>
+      </c>
+      <c r="C156" t="s">
+        <v>34</v>
+      </c>
+      <c r="D156" t="s">
+        <v>191</v>
+      </c>
+      <c r="E156" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>139</v>
+      </c>
+      <c r="B157" t="s">
+        <v>66</v>
+      </c>
+      <c r="C157" t="s">
+        <v>36</v>
+      </c>
+      <c r="D157" t="s">
+        <v>193</v>
+      </c>
+      <c r="E157" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix synapse IDs for CRC data
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laveryj\Desktop\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EF6F4F-C646-42CA-A2B0-809275257C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7A869A-A8D0-4CB3-B70B-5C51CB470723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$158</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -327,36 +330,9 @@
     <t>2020-10</t>
   </si>
   <si>
-    <t>syn39802294</t>
-  </si>
-  <si>
     <t>2022-10</t>
   </si>
   <si>
-    <t>syn39802300</t>
-  </si>
-  <si>
-    <t>syn39802305</t>
-  </si>
-  <si>
-    <t>syn39802310</t>
-  </si>
-  <si>
-    <t>syn39802316</t>
-  </si>
-  <si>
-    <t>syn39802321</t>
-  </si>
-  <si>
-    <t>syn39802324</t>
-  </si>
-  <si>
-    <t>syn39802332</t>
-  </si>
-  <si>
-    <t>syn39802339</t>
-  </si>
-  <si>
     <t>2022-11</t>
   </si>
   <si>
@@ -525,15 +501,6 @@
     <t>syn43172837</t>
   </si>
   <si>
-    <t>syn30381335</t>
-  </si>
-  <si>
-    <t>syn30381332</t>
-  </si>
-  <si>
-    <t>syn30381327</t>
-  </si>
-  <si>
     <t>syn26349094</t>
   </si>
   <si>
@@ -616,6 +583,42 @@
   </si>
   <si>
     <t>syn50895310</t>
+  </si>
+  <si>
+    <t>syn39802589</t>
+  </si>
+  <si>
+    <t>syn39802574</t>
+  </si>
+  <si>
+    <t>syn39802575</t>
+  </si>
+  <si>
+    <t>syn39802578</t>
+  </si>
+  <si>
+    <t>syn39802579</t>
+  </si>
+  <si>
+    <t>syn39802583</t>
+  </si>
+  <si>
+    <t>syn39802586</t>
+  </si>
+  <si>
+    <t>syn39802591</t>
+  </si>
+  <si>
+    <t>syn39802593</t>
+  </si>
+  <si>
+    <t>syn39802627</t>
+  </si>
+  <si>
+    <t>syn39802604</t>
+  </si>
+  <si>
+    <t>syn39802596</t>
   </si>
 </sst>
 </file>
@@ -985,21 +988,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
   <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1832,7 +1835,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -2200,13 +2203,13 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
+        <v>184</v>
+      </c>
+      <c r="E71" t="s">
         <v>98</v>
       </c>
-      <c r="E71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -2217,13 +2220,13 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="E72" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -2234,13 +2237,13 @@
         <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -2251,13 +2254,13 @@
         <v>8</v>
       </c>
       <c r="D74" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2268,13 +2271,13 @@
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="E75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2285,13 +2288,13 @@
         <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="E76" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2302,13 +2305,13 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="E77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -2319,13 +2322,13 @@
         <v>11</v>
       </c>
       <c r="D78" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2336,13 +2339,13 @@
         <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
       <c r="E79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>52</v>
       </c>
@@ -2353,13 +2356,13 @@
         <v>32</v>
       </c>
       <c r="D80" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E80" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>52</v>
       </c>
@@ -2370,13 +2373,13 @@
         <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="E81" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -2387,15 +2390,15 @@
         <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="E82" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
@@ -2404,15 +2407,15 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B84" t="s">
         <v>22</v>
@@ -2421,15 +2424,15 @@
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E84" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
         <v>22</v>
@@ -2438,15 +2441,15 @@
         <v>12</v>
       </c>
       <c r="D85" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E85" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
         <v>22</v>
@@ -2455,15 +2458,15 @@
         <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E86" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
         <v>22</v>
@@ -2472,15 +2475,15 @@
         <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E87" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
         <v>22</v>
@@ -2489,15 +2492,15 @@
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B89" t="s">
         <v>22</v>
@@ -2506,15 +2509,15 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E89" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B90" t="s">
         <v>22</v>
@@ -2523,32 +2526,32 @@
         <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E90" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D91" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E91" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
         <v>22</v>
@@ -2557,15 +2560,15 @@
         <v>53</v>
       </c>
       <c r="D92" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E92" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
@@ -2574,15 +2577,15 @@
         <v>32</v>
       </c>
       <c r="D93" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E93" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
@@ -2591,15 +2594,15 @@
         <v>34</v>
       </c>
       <c r="D94" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E94" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B95" t="s">
         <v>22</v>
@@ -2608,32 +2611,32 @@
         <v>36</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E95" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
         <v>110</v>
       </c>
-      <c r="B96" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" t="s">
-        <v>119</v>
-      </c>
       <c r="D96" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E96" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B97" t="s">
         <v>22</v>
@@ -2642,15 +2645,15 @@
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
@@ -2659,15 +2662,15 @@
         <v>7</v>
       </c>
       <c r="D98" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E98" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
         <v>22</v>
@@ -2676,15 +2679,15 @@
         <v>12</v>
       </c>
       <c r="D99" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E99" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
         <v>22</v>
@@ -2693,15 +2696,15 @@
         <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E100" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>22</v>
@@ -2710,15 +2713,15 @@
         <v>10</v>
       </c>
       <c r="D101" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E101" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>22</v>
@@ -2727,15 +2730,15 @@
         <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E102" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>22</v>
@@ -2744,15 +2747,15 @@
         <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E103" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
         <v>22</v>
@@ -2761,15 +2764,15 @@
         <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E104" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
         <v>22</v>
@@ -2778,15 +2781,15 @@
         <v>32</v>
       </c>
       <c r="D105" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B106" t="s">
         <v>22</v>
@@ -2795,15 +2798,15 @@
         <v>34</v>
       </c>
       <c r="D106" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E106" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B107" t="s">
         <v>22</v>
@@ -2812,13 +2815,13 @@
         <v>36</v>
       </c>
       <c r="D107" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>79</v>
       </c>
@@ -2829,13 +2832,13 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E108" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>79</v>
       </c>
@@ -2846,13 +2849,13 @@
         <v>7</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E109" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>79</v>
       </c>
@@ -2863,13 +2866,13 @@
         <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E110" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>79</v>
       </c>
@@ -2880,13 +2883,13 @@
         <v>8</v>
       </c>
       <c r="D111" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E111" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>79</v>
       </c>
@@ -2897,13 +2900,13 @@
         <v>10</v>
       </c>
       <c r="D112" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E112" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>79</v>
       </c>
@@ -2914,13 +2917,13 @@
         <v>9</v>
       </c>
       <c r="D113" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E113" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>79</v>
       </c>
@@ -2931,13 +2934,13 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E114" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>79</v>
       </c>
@@ -2948,13 +2951,13 @@
         <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E115" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -2965,13 +2968,13 @@
         <v>53</v>
       </c>
       <c r="D116" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E116" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>79</v>
       </c>
@@ -2982,13 +2985,13 @@
         <v>32</v>
       </c>
       <c r="D117" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E117" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -2999,13 +3002,13 @@
         <v>34</v>
       </c>
       <c r="D118" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E118" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>79</v>
       </c>
@@ -3016,32 +3019,32 @@
         <v>36</v>
       </c>
       <c r="D119" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E119" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B120" t="s">
         <v>22</v>
       </c>
       <c r="C120" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D120" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E120" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B121" t="s">
         <v>22</v>
@@ -3050,15 +3053,15 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E121" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>22</v>
@@ -3067,15 +3070,15 @@
         <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E122" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>22</v>
@@ -3084,15 +3087,15 @@
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E123" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
         <v>22</v>
@@ -3101,15 +3104,15 @@
         <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E124" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
         <v>22</v>
@@ -3118,15 +3121,15 @@
         <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E125" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B126" t="s">
         <v>22</v>
@@ -3135,15 +3138,15 @@
         <v>9</v>
       </c>
       <c r="D126" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E126" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B127" t="s">
         <v>22</v>
@@ -3152,15 +3155,15 @@
         <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E127" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B128" t="s">
         <v>22</v>
@@ -3169,15 +3172,15 @@
         <v>11</v>
       </c>
       <c r="D128" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E128" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B129" t="s">
         <v>22</v>
@@ -3186,15 +3189,15 @@
         <v>53</v>
       </c>
       <c r="D129" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E129" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B130" t="s">
         <v>22</v>
@@ -3203,15 +3206,15 @@
         <v>32</v>
       </c>
       <c r="D130" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E130" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B131" t="s">
         <v>22</v>
@@ -3220,15 +3223,15 @@
         <v>34</v>
       </c>
       <c r="D131" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E131" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B132" t="s">
         <v>22</v>
@@ -3237,32 +3240,32 @@
         <v>36</v>
       </c>
       <c r="D132" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E132" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B133" t="s">
         <v>66</v>
       </c>
       <c r="C133" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D133" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E133" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B134" t="s">
         <v>66</v>
@@ -3271,15 +3274,15 @@
         <v>6</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E134" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B135" t="s">
         <v>66</v>
@@ -3288,15 +3291,15 @@
         <v>7</v>
       </c>
       <c r="D135" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E135" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B136" t="s">
         <v>66</v>
@@ -3305,15 +3308,15 @@
         <v>12</v>
       </c>
       <c r="D136" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E136" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B137" t="s">
         <v>66</v>
@@ -3322,15 +3325,15 @@
         <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E137" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B138" t="s">
         <v>66</v>
@@ -3339,15 +3342,15 @@
         <v>10</v>
       </c>
       <c r="D138" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E138" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B139" t="s">
         <v>66</v>
@@ -3356,15 +3359,15 @@
         <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E139" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B140" t="s">
         <v>66</v>
@@ -3373,15 +3376,15 @@
         <v>5</v>
       </c>
       <c r="D140" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E140" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B141" t="s">
         <v>66</v>
@@ -3390,15 +3393,15 @@
         <v>11</v>
       </c>
       <c r="D141" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E141" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B142" t="s">
         <v>66</v>
@@ -3407,15 +3410,15 @@
         <v>53</v>
       </c>
       <c r="D142" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E142" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B143" t="s">
         <v>66</v>
@@ -3424,15 +3427,15 @@
         <v>32</v>
       </c>
       <c r="D143" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E143" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B144" t="s">
         <v>66</v>
@@ -3441,15 +3444,15 @@
         <v>34</v>
       </c>
       <c r="D144" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E144" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B145" t="s">
         <v>66</v>
@@ -3458,32 +3461,32 @@
         <v>36</v>
       </c>
       <c r="D145" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E145" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B146" t="s">
         <v>66</v>
       </c>
       <c r="C146" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D146" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E146" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B147" t="s">
         <v>66</v>
@@ -3492,15 +3495,15 @@
         <v>6</v>
       </c>
       <c r="D147" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E147" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B148" t="s">
         <v>66</v>
@@ -3509,15 +3512,15 @@
         <v>7</v>
       </c>
       <c r="D148" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E148" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B149" t="s">
         <v>66</v>
@@ -3526,15 +3529,15 @@
         <v>12</v>
       </c>
       <c r="D149" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E149" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B150" t="s">
         <v>66</v>
@@ -3543,15 +3546,15 @@
         <v>8</v>
       </c>
       <c r="D150" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E150" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B151" t="s">
         <v>66</v>
@@ -3560,15 +3563,15 @@
         <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E151" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B152" t="s">
         <v>66</v>
@@ -3577,15 +3580,15 @@
         <v>9</v>
       </c>
       <c r="D152" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E152" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B153" t="s">
         <v>66</v>
@@ -3594,15 +3597,15 @@
         <v>5</v>
       </c>
       <c r="D153" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E153" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B154" t="s">
         <v>66</v>
@@ -3611,15 +3614,15 @@
         <v>11</v>
       </c>
       <c r="D154" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E154" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B155" t="s">
         <v>66</v>
@@ -3628,15 +3631,15 @@
         <v>53</v>
       </c>
       <c r="D155" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E155" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
         <v>66</v>
@@ -3645,15 +3648,15 @@
         <v>32</v>
       </c>
       <c r="D156" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E156" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B157" t="s">
         <v>66</v>
@@ -3662,15 +3665,15 @@
         <v>34</v>
       </c>
       <c r="D157" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E157" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B158" t="s">
         <v>66</v>
@@ -3679,13 +3682,14 @@
         <v>36</v>
       </c>
       <c r="D158" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E158" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E158" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix synapse IDs for CRC data (#107)
</commit_message>
<xml_diff>
--- a/data-raw/synapse_tables.xlsx
+++ b/data-raw/synapse_tables.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laveryj\Desktop\genieBPC\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EF6F4F-C646-42CA-A2B0-809275257C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7A869A-A8D0-4CB3-B70B-5C51CB470723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BE4D035A-8EA9-486C-93EE-A0673DF8CE94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$158</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -327,36 +330,9 @@
     <t>2020-10</t>
   </si>
   <si>
-    <t>syn39802294</t>
-  </si>
-  <si>
     <t>2022-10</t>
   </si>
   <si>
-    <t>syn39802300</t>
-  </si>
-  <si>
-    <t>syn39802305</t>
-  </si>
-  <si>
-    <t>syn39802310</t>
-  </si>
-  <si>
-    <t>syn39802316</t>
-  </si>
-  <si>
-    <t>syn39802321</t>
-  </si>
-  <si>
-    <t>syn39802324</t>
-  </si>
-  <si>
-    <t>syn39802332</t>
-  </si>
-  <si>
-    <t>syn39802339</t>
-  </si>
-  <si>
     <t>2022-11</t>
   </si>
   <si>
@@ -525,15 +501,6 @@
     <t>syn43172837</t>
   </si>
   <si>
-    <t>syn30381335</t>
-  </si>
-  <si>
-    <t>syn30381332</t>
-  </si>
-  <si>
-    <t>syn30381327</t>
-  </si>
-  <si>
     <t>syn26349094</t>
   </si>
   <si>
@@ -616,6 +583,42 @@
   </si>
   <si>
     <t>syn50895310</t>
+  </si>
+  <si>
+    <t>syn39802589</t>
+  </si>
+  <si>
+    <t>syn39802574</t>
+  </si>
+  <si>
+    <t>syn39802575</t>
+  </si>
+  <si>
+    <t>syn39802578</t>
+  </si>
+  <si>
+    <t>syn39802579</t>
+  </si>
+  <si>
+    <t>syn39802583</t>
+  </si>
+  <si>
+    <t>syn39802586</t>
+  </si>
+  <si>
+    <t>syn39802591</t>
+  </si>
+  <si>
+    <t>syn39802593</t>
+  </si>
+  <si>
+    <t>syn39802627</t>
+  </si>
+  <si>
+    <t>syn39802604</t>
+  </si>
+  <si>
+    <t>syn39802596</t>
   </si>
 </sst>
 </file>
@@ -985,21 +988,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}">
   <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1019,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1101,7 +1104,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1342,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1475,7 +1478,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1594,7 +1597,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1781,7 +1784,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1798,7 +1801,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1832,7 +1835,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -2070,7 +2073,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>52</v>
       </c>
@@ -2200,13 +2203,13 @@
         <v>6</v>
       </c>
       <c r="D71" t="s">
+        <v>184</v>
+      </c>
+      <c r="E71" t="s">
         <v>98</v>
       </c>
-      <c r="E71" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -2217,13 +2220,13 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="E72" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>52</v>
       </c>
@@ -2234,13 +2237,13 @@
         <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>186</v>
       </c>
       <c r="E73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>52</v>
       </c>
@@ -2251,13 +2254,13 @@
         <v>8</v>
       </c>
       <c r="D74" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="E74" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>52</v>
       </c>
@@ -2268,13 +2271,13 @@
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>103</v>
+        <v>188</v>
       </c>
       <c r="E75" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2285,13 +2288,13 @@
         <v>9</v>
       </c>
       <c r="D76" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="E76" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -2302,13 +2305,13 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="E77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -2319,13 +2322,13 @@
         <v>11</v>
       </c>
       <c r="D78" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2336,13 +2339,13 @@
         <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
       <c r="E79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>52</v>
       </c>
@@ -2353,13 +2356,13 @@
         <v>32</v>
       </c>
       <c r="D80" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="E80" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>52</v>
       </c>
@@ -2370,13 +2373,13 @@
         <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="E81" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>52</v>
       </c>
@@ -2387,15 +2390,15 @@
         <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="E82" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
@@ -2404,15 +2407,15 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B84" t="s">
         <v>22</v>
@@ -2421,15 +2424,15 @@
         <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E84" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B85" t="s">
         <v>22</v>
@@ -2438,15 +2441,15 @@
         <v>12</v>
       </c>
       <c r="D85" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="E85" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B86" t="s">
         <v>22</v>
@@ -2455,15 +2458,15 @@
         <v>8</v>
       </c>
       <c r="D86" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E86" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B87" t="s">
         <v>22</v>
@@ -2472,15 +2475,15 @@
         <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E87" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
         <v>22</v>
@@ -2489,15 +2492,15 @@
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="E88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B89" t="s">
         <v>22</v>
@@ -2506,15 +2509,15 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E89" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B90" t="s">
         <v>22</v>
@@ -2523,32 +2526,32 @@
         <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="E90" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B91" t="s">
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D91" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="E91" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
         <v>22</v>
@@ -2557,15 +2560,15 @@
         <v>53</v>
       </c>
       <c r="D92" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="E92" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
@@ -2574,15 +2577,15 @@
         <v>32</v>
       </c>
       <c r="D93" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="E93" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
@@ -2591,15 +2594,15 @@
         <v>34</v>
       </c>
       <c r="D94" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E94" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B95" t="s">
         <v>22</v>
@@ -2608,32 +2611,32 @@
         <v>36</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="E95" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
         <v>110</v>
       </c>
-      <c r="B96" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" t="s">
-        <v>119</v>
-      </c>
       <c r="D96" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E96" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B97" t="s">
         <v>22</v>
@@ -2642,15 +2645,15 @@
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="E97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B98" t="s">
         <v>22</v>
@@ -2659,15 +2662,15 @@
         <v>7</v>
       </c>
       <c r="D98" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E98" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
         <v>22</v>
@@ -2676,15 +2679,15 @@
         <v>12</v>
       </c>
       <c r="D99" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E99" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
         <v>22</v>
@@ -2693,15 +2696,15 @@
         <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E100" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>22</v>
@@ -2710,15 +2713,15 @@
         <v>10</v>
       </c>
       <c r="D101" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E101" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>22</v>
@@ -2727,15 +2730,15 @@
         <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E102" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>22</v>
@@ -2744,15 +2747,15 @@
         <v>5</v>
       </c>
       <c r="D103" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E103" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
         <v>22</v>
@@ -2761,15 +2764,15 @@
         <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E104" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
         <v>22</v>
@@ -2778,15 +2781,15 @@
         <v>32</v>
       </c>
       <c r="D105" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E105" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B106" t="s">
         <v>22</v>
@@ -2795,15 +2798,15 @@
         <v>34</v>
       </c>
       <c r="D106" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E106" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B107" t="s">
         <v>22</v>
@@ -2812,13 +2815,13 @@
         <v>36</v>
       </c>
       <c r="D107" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E107" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>79</v>
       </c>
@@ -2829,13 +2832,13 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="E108" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>79</v>
       </c>
@@ -2846,13 +2849,13 @@
         <v>7</v>
       </c>
       <c r="D109" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E109" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>79</v>
       </c>
@@ -2863,13 +2866,13 @@
         <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E110" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>79</v>
       </c>
@@ -2880,13 +2883,13 @@
         <v>8</v>
       </c>
       <c r="D111" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E111" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>79</v>
       </c>
@@ -2897,13 +2900,13 @@
         <v>10</v>
       </c>
       <c r="D112" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E112" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>79</v>
       </c>
@@ -2914,13 +2917,13 @@
         <v>9</v>
       </c>
       <c r="D113" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E113" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>79</v>
       </c>
@@ -2931,13 +2934,13 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E114" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>79</v>
       </c>
@@ -2948,13 +2951,13 @@
         <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E115" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>79</v>
       </c>
@@ -2965,13 +2968,13 @@
         <v>53</v>
       </c>
       <c r="D116" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="E116" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>79</v>
       </c>
@@ -2982,13 +2985,13 @@
         <v>32</v>
       </c>
       <c r="D117" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E117" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -2999,13 +3002,13 @@
         <v>34</v>
       </c>
       <c r="D118" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E118" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>79</v>
       </c>
@@ -3016,32 +3019,32 @@
         <v>36</v>
       </c>
       <c r="D119" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E119" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B120" t="s">
         <v>22</v>
       </c>
       <c r="C120" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D120" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="E120" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B121" t="s">
         <v>22</v>
@@ -3050,15 +3053,15 @@
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="E121" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>22</v>
@@ -3067,15 +3070,15 @@
         <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="E122" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>22</v>
@@ -3084,15 +3087,15 @@
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E123" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
         <v>22</v>
@@ -3101,15 +3104,15 @@
         <v>8</v>
       </c>
       <c r="D124" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="E124" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B125" t="s">
         <v>22</v>
@@ -3118,15 +3121,15 @@
         <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E125" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B126" t="s">
         <v>22</v>
@@ -3135,15 +3138,15 @@
         <v>9</v>
       </c>
       <c r="D126" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="E126" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B127" t="s">
         <v>22</v>
@@ -3152,15 +3155,15 @@
         <v>5</v>
       </c>
       <c r="D127" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E127" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B128" t="s">
         <v>22</v>
@@ -3169,15 +3172,15 @@
         <v>11</v>
       </c>
       <c r="D128" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E128" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B129" t="s">
         <v>22</v>
@@ -3186,15 +3189,15 @@
         <v>53</v>
       </c>
       <c r="D129" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E129" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B130" t="s">
         <v>22</v>
@@ -3203,15 +3206,15 @@
         <v>32</v>
       </c>
       <c r="D130" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E130" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B131" t="s">
         <v>22</v>
@@ -3220,15 +3223,15 @@
         <v>34</v>
       </c>
       <c r="D131" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E131" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B132" t="s">
         <v>22</v>
@@ -3237,32 +3240,32 @@
         <v>36</v>
       </c>
       <c r="D132" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E132" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B133" t="s">
         <v>66</v>
       </c>
       <c r="C133" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D133" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E133" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B134" t="s">
         <v>66</v>
@@ -3271,15 +3274,15 @@
         <v>6</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E134" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B135" t="s">
         <v>66</v>
@@ -3288,15 +3291,15 @@
         <v>7</v>
       </c>
       <c r="D135" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E135" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B136" t="s">
         <v>66</v>
@@ -3305,15 +3308,15 @@
         <v>12</v>
       </c>
       <c r="D136" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E136" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B137" t="s">
         <v>66</v>
@@ -3322,15 +3325,15 @@
         <v>8</v>
       </c>
       <c r="D137" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E137" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B138" t="s">
         <v>66</v>
@@ -3339,15 +3342,15 @@
         <v>10</v>
       </c>
       <c r="D138" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E138" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B139" t="s">
         <v>66</v>
@@ -3356,15 +3359,15 @@
         <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E139" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B140" t="s">
         <v>66</v>
@@ -3373,15 +3376,15 @@
         <v>5</v>
       </c>
       <c r="D140" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E140" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B141" t="s">
         <v>66</v>
@@ -3390,15 +3393,15 @@
         <v>11</v>
       </c>
       <c r="D141" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E141" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B142" t="s">
         <v>66</v>
@@ -3407,15 +3410,15 @@
         <v>53</v>
       </c>
       <c r="D142" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E142" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B143" t="s">
         <v>66</v>
@@ -3424,15 +3427,15 @@
         <v>32</v>
       </c>
       <c r="D143" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E143" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B144" t="s">
         <v>66</v>
@@ -3441,15 +3444,15 @@
         <v>34</v>
       </c>
       <c r="D144" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E144" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B145" t="s">
         <v>66</v>
@@ -3458,32 +3461,32 @@
         <v>36</v>
       </c>
       <c r="D145" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E145" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B146" t="s">
         <v>66</v>
       </c>
       <c r="C146" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D146" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E146" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B147" t="s">
         <v>66</v>
@@ -3492,15 +3495,15 @@
         <v>6</v>
       </c>
       <c r="D147" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E147" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B148" t="s">
         <v>66</v>
@@ -3509,15 +3512,15 @@
         <v>7</v>
       </c>
       <c r="D148" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E148" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B149" t="s">
         <v>66</v>
@@ -3526,15 +3529,15 @@
         <v>12</v>
       </c>
       <c r="D149" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="E149" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B150" t="s">
         <v>66</v>
@@ -3543,15 +3546,15 @@
         <v>8</v>
       </c>
       <c r="D150" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E150" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B151" t="s">
         <v>66</v>
@@ -3560,15 +3563,15 @@
         <v>10</v>
       </c>
       <c r="D151" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E151" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B152" t="s">
         <v>66</v>
@@ -3577,15 +3580,15 @@
         <v>9</v>
       </c>
       <c r="D152" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="E152" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B153" t="s">
         <v>66</v>
@@ -3594,15 +3597,15 @@
         <v>5</v>
       </c>
       <c r="D153" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E153" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B154" t="s">
         <v>66</v>
@@ -3611,15 +3614,15 @@
         <v>11</v>
       </c>
       <c r="D154" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E154" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B155" t="s">
         <v>66</v>
@@ -3628,15 +3631,15 @@
         <v>53</v>
       </c>
       <c r="D155" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E155" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
         <v>66</v>
@@ -3645,15 +3648,15 @@
         <v>32</v>
       </c>
       <c r="D156" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E156" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B157" t="s">
         <v>66</v>
@@ -3662,15 +3665,15 @@
         <v>34</v>
       </c>
       <c r="D157" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E157" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B158" t="s">
         <v>66</v>
@@ -3679,13 +3682,14 @@
         <v>36</v>
       </c>
       <c r="D158" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E158" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E158" xr:uid="{ABC6D6DE-1343-424E-9447-2DE3FE58E3B9}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>